<commit_message>
Added BOM files for sensor, AC-DC and top level
</commit_message>
<xml_diff>
--- a/mfg/BOM/bom-Vayu-R1A.xlsx
+++ b/mfg/BOM/bom-Vayu-R1A.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varun\Documents\EAGLE\projects\Vayu\mfg\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C811F3B-A165-4ED7-B169-5F0FDA698B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44607DAD-25B3-479E-8507-AE9D32E2749A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" activeTab="1" xr2:uid="{2AC65B7F-617A-40F0-94CF-F2A301846D0E}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{2AC65B7F-617A-40F0-94CF-F2A301846D0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="2" r:id="rId1"/>
@@ -264,9 +264,6 @@
     <t>Vayu</t>
   </si>
   <si>
-    <t>bom-Vayu</t>
-  </si>
-  <si>
     <t>PCBA-Vayu-R1A</t>
   </si>
   <si>
@@ -550,6 +547,9 @@
   </si>
   <si>
     <t>CAPACITOR, C0G NP0, 50V, 1%, SMT, RoHS</t>
+  </si>
+  <si>
+    <t>bom-Vayu-R1A</t>
   </si>
 </sst>
 </file>
@@ -1094,7 +1094,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1102,17 +1102,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1531,8 +1530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE2DABB5-3332-44BC-A0AE-4D5C4D708176}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1563,7 +1562,7 @@
         <v>56</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>76</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.35">
@@ -1587,7 +1586,7 @@
         <v>61</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1596,46 +1595,46 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
@@ -1649,33 +1648,33 @@
       <c r="A17" s="4"/>
     </row>
     <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="8" t="s">
+      <c r="B18" s="10"/>
+      <c r="C18" s="5" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="6" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="7" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1697,7 +1696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{479BCEB5-D3BA-4242-B9D5-86AA0632D7C9}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -1716,62 +1715,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="str">
+      <c r="A1" s="12" t="str">
         <f>CONCATENATE("Marolia"," - Compressed sheet - ","Project: ",Information!B2,", Doc: ",Information!B3,", Rev: ",Information!B4,", Date: ",Information!B5)</f>
-        <v>Marolia - Compressed sheet - Project: Vayu, Doc: bom-Vayu, Rev: A, Date: Oct/01/2024</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
+        <v>Marolia - Compressed sheet - Project: Vayu, Doc: bom-Vayu-R1A, Rev: A, Date: Oct/01/2024</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="12" t="s">
+      <c r="F2" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="G2" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="H2" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="I2" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="J2" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="K2" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="L2" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="M2" s="8" t="s">
         <v>97</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1779,7 +1778,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -1788,25 +1787,25 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G3" t="s">
+        <v>109</v>
+      </c>
+      <c r="H3" t="s">
         <v>110</v>
       </c>
-      <c r="H3" t="s">
-        <v>111</v>
-      </c>
       <c r="I3" t="s">
+        <v>120</v>
+      </c>
+      <c r="J3" t="s">
+        <v>113</v>
+      </c>
+      <c r="K3" t="s">
         <v>121</v>
-      </c>
-      <c r="J3" t="s">
-        <v>114</v>
-      </c>
-      <c r="K3" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1814,7 +1813,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -1823,25 +1822,25 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G4" t="s">
+        <v>109</v>
+      </c>
+      <c r="H4" t="s">
         <v>110</v>
       </c>
-      <c r="H4" t="s">
-        <v>111</v>
-      </c>
       <c r="I4" t="s">
+        <v>115</v>
+      </c>
+      <c r="J4" t="s">
+        <v>113</v>
+      </c>
+      <c r="K4" t="s">
         <v>116</v>
-      </c>
-      <c r="J4" t="s">
-        <v>114</v>
-      </c>
-      <c r="K4" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1849,7 +1848,7 @@
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -1858,25 +1857,25 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G5" t="s">
+        <v>109</v>
+      </c>
+      <c r="H5" t="s">
         <v>110</v>
       </c>
-      <c r="H5" t="s">
-        <v>111</v>
-      </c>
       <c r="I5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J5" t="s">
+        <v>113</v>
+      </c>
+      <c r="K5" t="s">
         <v>118</v>
-      </c>
-      <c r="J5" t="s">
-        <v>114</v>
-      </c>
-      <c r="K5" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1884,7 +1883,7 @@
         <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -1893,25 +1892,25 @@
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G6" t="s">
+        <v>109</v>
+      </c>
+      <c r="H6" t="s">
         <v>110</v>
       </c>
-      <c r="H6" t="s">
-        <v>111</v>
-      </c>
       <c r="I6" t="s">
+        <v>159</v>
+      </c>
+      <c r="J6" t="s">
         <v>160</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>161</v>
-      </c>
-      <c r="K6" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1919,7 +1918,7 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -1931,16 +1930,16 @@
         <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H7" t="s">
         <v>110</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>111</v>
-      </c>
-      <c r="I7" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1948,7 +1947,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -1957,33 +1956,33 @@
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H8" t="s">
         <v>110</v>
       </c>
-      <c r="H8" t="s">
-        <v>111</v>
-      </c>
       <c r="I8" t="s">
+        <v>112</v>
+      </c>
+      <c r="J8" t="s">
         <v>113</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>114</v>
-      </c>
-      <c r="K8" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" t="s">
         <v>101</v>
-      </c>
-      <c r="B9" t="s">
-        <v>102</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -1995,16 +1994,16 @@
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -2012,7 +2011,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
@@ -2021,25 +2020,25 @@
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I10" t="s">
+        <v>123</v>
+      </c>
+      <c r="J10" t="s">
+        <v>113</v>
+      </c>
+      <c r="K10" t="s">
         <v>124</v>
-      </c>
-      <c r="J10" t="s">
-        <v>114</v>
-      </c>
-      <c r="K10" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -2047,34 +2046,34 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G11" t="s">
+        <v>109</v>
+      </c>
+      <c r="H11" t="s">
+        <v>102</v>
+      </c>
+      <c r="I11" t="s">
+        <v>157</v>
+      </c>
+      <c r="J11" t="s">
         <v>110</v>
       </c>
-      <c r="H11" t="s">
-        <v>103</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="K11" t="s">
         <v>158</v>
-      </c>
-      <c r="J11" t="s">
-        <v>111</v>
-      </c>
-      <c r="K11" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -2082,7 +2081,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -2091,25 +2090,25 @@
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J12" t="s">
+        <v>113</v>
+      </c>
+      <c r="K12" t="s">
         <v>126</v>
-      </c>
-      <c r="J12" t="s">
-        <v>114</v>
-      </c>
-      <c r="K12" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -2117,7 +2116,7 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
@@ -2129,22 +2128,22 @@
         <v>24</v>
       </c>
       <c r="F13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I13" t="s">
+        <v>155</v>
+      </c>
+      <c r="J13" t="s">
+        <v>113</v>
+      </c>
+      <c r="K13" t="s">
         <v>156</v>
-      </c>
-      <c r="J13" t="s">
-        <v>114</v>
-      </c>
-      <c r="K13" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -2152,7 +2151,7 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -2161,25 +2160,25 @@
         <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I14" t="s">
+        <v>127</v>
+      </c>
+      <c r="J14" t="s">
+        <v>113</v>
+      </c>
+      <c r="K14" t="s">
         <v>128</v>
-      </c>
-      <c r="J14" t="s">
-        <v>114</v>
-      </c>
-      <c r="K14" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -2187,7 +2186,7 @@
         <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C15" t="s">
         <v>43</v>
@@ -2199,19 +2198,19 @@
         <v>44</v>
       </c>
       <c r="F15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I15" t="s">
         <v>42</v>
       </c>
       <c r="J15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K15" t="s">
         <v>42</v>
@@ -2222,7 +2221,7 @@
         <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C16" t="s">
         <v>32</v>
@@ -2234,22 +2233,22 @@
         <v>33</v>
       </c>
       <c r="F16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I16" t="s">
         <v>31</v>
       </c>
       <c r="J16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2257,7 +2256,7 @@
         <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C17" t="s">
         <v>35</v>
@@ -2269,30 +2268,30 @@
         <v>36</v>
       </c>
       <c r="F17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I17" t="s">
         <v>34</v>
       </c>
       <c r="J17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>163</v>
+      <c r="A18" t="s">
+        <v>162</v>
       </c>
       <c r="B18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C18" t="s">
         <v>13</v>
@@ -2301,16 +2300,16 @@
         <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G18" t="s">
         <v>58</v>
       </c>
       <c r="H18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I18">
         <v>1770911</v>
@@ -2321,7 +2320,7 @@
         <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C19" t="s">
         <v>27</v>
@@ -2333,13 +2332,13 @@
         <v>28</v>
       </c>
       <c r="F19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G19" t="s">
         <v>58</v>
       </c>
       <c r="H19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I19" t="s">
         <v>26</v>
@@ -2350,7 +2349,7 @@
         <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C20" t="s">
         <v>40</v>
@@ -2362,16 +2361,16 @@
         <v>41</v>
       </c>
       <c r="F20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G20" t="s">
         <v>58</v>
       </c>
       <c r="H20" t="s">
+        <v>144</v>
+      </c>
+      <c r="I20" t="s">
         <v>145</v>
-      </c>
-      <c r="I20" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -2379,7 +2378,7 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C21" t="s">
         <v>18</v>
@@ -2391,22 +2390,22 @@
         <v>19</v>
       </c>
       <c r="F21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I21" t="s">
         <v>17</v>
       </c>
       <c r="J21" t="s">
+        <v>168</v>
+      </c>
+      <c r="K21" t="s">
         <v>169</v>
-      </c>
-      <c r="K21" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -2414,7 +2413,7 @@
         <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C22" t="s">
         <v>38</v>
@@ -2423,25 +2422,25 @@
         <v>4</v>
       </c>
       <c r="E22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H22" t="s">
+        <v>129</v>
+      </c>
+      <c r="I22" t="s">
         <v>130</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>131</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>132</v>
-      </c>
-      <c r="K22" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -2449,7 +2448,7 @@
         <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C23" t="s">
         <v>46</v>
@@ -2458,16 +2457,16 @@
         <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I23" t="s">
         <v>45</v>
@@ -2478,7 +2477,7 @@
         <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C24" t="s">
         <v>51</v>
@@ -2490,16 +2489,16 @@
         <v>52</v>
       </c>
       <c r="F24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G24" t="s">
         <v>58</v>
       </c>
       <c r="H24" t="s">
+        <v>137</v>
+      </c>
+      <c r="I24" t="s">
         <v>138</v>
-      </c>
-      <c r="I24" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -2507,7 +2506,7 @@
         <v>47</v>
       </c>
       <c r="B25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C25" t="s">
         <v>48</v>
@@ -2519,13 +2518,13 @@
         <v>49</v>
       </c>
       <c r="F25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G25" t="s">
         <v>58</v>
       </c>
       <c r="H25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I25" t="s">
         <v>47</v>
@@ -2536,7 +2535,7 @@
         <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C26" t="s">
         <v>30</v>
@@ -2545,16 +2544,16 @@
         <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I26" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
bug fix, updated MOSFET driver and other MOSFETS, added SWO support
</commit_message>
<xml_diff>
--- a/mfg/BOM/bom-Vayu-R1A.xlsx
+++ b/mfg/BOM/bom-Vayu-R1A.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varun\Documents\EAGLE\projects\Vayu\mfg\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44607DAD-25B3-479E-8507-AE9D32E2749A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E25CAA-44E8-4F26-8B80-7534BDE1A674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{2AC65B7F-617A-40F0-94CF-F2A301846D0E}"/>
+    <workbookView xWindow="5880" yWindow="1680" windowWidth="38700" windowHeight="15345" activeTab="1" xr2:uid="{2AC65B7F-617A-40F0-94CF-F2A301846D0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="185">
   <si>
     <t>Qty</t>
   </si>
@@ -99,9 +99,6 @@
     <t>200K</t>
   </si>
   <si>
-    <t>R7</t>
-  </si>
-  <si>
     <t>220E</t>
   </si>
   <si>
@@ -111,9 +108,6 @@
     <t>C6</t>
   </si>
   <si>
-    <t>300K</t>
-  </si>
-  <si>
     <t>3220-10-0100-00</t>
   </si>
   <si>
@@ -168,9 +162,6 @@
     <t>SOD-123F-BI</t>
   </si>
   <si>
-    <t>D1</t>
-  </si>
-  <si>
     <t>TL1105LF160Q</t>
   </si>
   <si>
@@ -270,9 +261,6 @@
     <t>C7, C8, C9, C10</t>
   </si>
   <si>
-    <t>R15, R16, R17</t>
-  </si>
-  <si>
     <t>C1, C3, C4</t>
   </si>
   <si>
@@ -282,24 +270,12 @@
     <t>J1, J2</t>
   </si>
   <si>
-    <t>R1, R2, R5</t>
-  </si>
-  <si>
-    <t>C2, C12</t>
-  </si>
-  <si>
     <t>R18, R19, R20, R21</t>
   </si>
   <si>
-    <t>R3, R4, R6</t>
-  </si>
-  <si>
     <t>V1, V2</t>
   </si>
   <si>
-    <t>Q1, Q2, Q3, Q4</t>
-  </si>
-  <si>
     <t>SW1, SW2</t>
   </si>
   <si>
@@ -393,9 +369,6 @@
     <t>RC1005F221CS</t>
   </si>
   <si>
-    <t>R8, R10, R11, R12, R13, R14</t>
-  </si>
-  <si>
     <t>RC0402FR-071ML</t>
   </si>
   <si>
@@ -513,15 +486,9 @@
     <t>AC0402FRNPO9BN102</t>
   </si>
   <si>
-    <t>RC0402FR-07300KL</t>
-  </si>
-  <si>
     <t>Bourns Inc.</t>
   </si>
   <si>
-    <t>CR0402-FX-3003GLF</t>
-  </si>
-  <si>
     <t>CON-1770911</t>
   </si>
   <si>
@@ -550,6 +517,78 @@
   </si>
   <si>
     <t>bom-Vayu-R1A</t>
+  </si>
+  <si>
+    <t>BSS138PW</t>
+  </si>
+  <si>
+    <t>MOSFET, N-Channel 60 V, 320 mA N-channel Trench MOSFET</t>
+  </si>
+  <si>
+    <t>SC-70</t>
+  </si>
+  <si>
+    <t>Q2,Q4</t>
+  </si>
+  <si>
+    <t>N-Channel 20 V 4A (Ta) 940mW Surface Mount SOT-23-3</t>
+  </si>
+  <si>
+    <t>DMN2056U-7</t>
+  </si>
+  <si>
+    <t>Nexperia USA Inc.</t>
+  </si>
+  <si>
+    <t>BSS138PW,115</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Bipolar (BJT) Transistor NPN 40 V 600 mA 250MHz 150 mW Surface Mount SC-70-3 (SOT323)</t>
+  </si>
+  <si>
+    <t>MMBT4401WT1G</t>
+  </si>
+  <si>
+    <t>Onsemi</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>R22, R10</t>
+  </si>
+  <si>
+    <t>47K</t>
+  </si>
+  <si>
+    <t>RC0402FR-1347KL</t>
+  </si>
+  <si>
+    <t>CR0402-FX-4702GLF</t>
+  </si>
+  <si>
+    <t>D1, D3</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R5, R3, R15, R16, R17, R23, R26</t>
+  </si>
+  <si>
+    <t>R7, R24</t>
+  </si>
+  <si>
+    <t>R1, R4, R6, R8, R11, R12, R13, R14, R25</t>
+  </si>
+  <si>
+    <t>C2, C12, C13, C14</t>
   </si>
 </sst>
 </file>
@@ -1190,8 +1229,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7547FB5C-F898-41B6-A398-D5D0AD2EC1A2}" name="Table1" displayName="Table1" ref="A2:M26" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A2:M26" xr:uid="{7547FB5C-F898-41B6-A398-D5D0AD2EC1A2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7547FB5C-F898-41B6-A398-D5D0AD2EC1A2}" name="Table1" displayName="Table1" ref="A2:M29" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A2:M29" xr:uid="{7547FB5C-F898-41B6-A398-D5D0AD2EC1A2}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{CADA81F9-76B1-4516-87BC-1C60C9F96761}" name="Value"/>
     <tableColumn id="2" xr3:uid="{7C962F1D-C975-45B4-9F5F-9A751599B25D}" name="Title"/>
@@ -1530,7 +1569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE2DABB5-3332-44BC-A0AE-4D5C4D708176}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1543,102 +1582,102 @@
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1649,33 +1688,33 @@
     </row>
     <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1694,10 +1733,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{479BCEB5-D3BA-4242-B9D5-86AA0632D7C9}">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1706,7 +1745,7 @@
     <col min="2" max="2" width="97.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="35.7109375" bestFit="1" customWidth="1"/>
@@ -1737,7 +1776,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>2</v>
@@ -1746,31 +1785,31 @@
         <v>0</v>
       </c>
       <c r="E2" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="L2" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>98</v>
-      </c>
       <c r="M2" s="8" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1778,34 +1817,34 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>82</v>
+        <v>180</v>
       </c>
       <c r="F3" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G3" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="H3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="I3" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="J3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="K3" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1813,42 +1852,42 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>78</v>
+        <v>181</v>
       </c>
       <c r="F4" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G4" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="H4" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="I4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="J4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="K4" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -1857,89 +1896,89 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="F5" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G5" t="s">
+        <v>101</v>
+      </c>
+      <c r="H5" t="s">
+        <v>102</v>
+      </c>
+      <c r="I5" t="s">
         <v>109</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
+        <v>105</v>
+      </c>
+      <c r="K5" t="s">
         <v>110</v>
-      </c>
-      <c r="I5" t="s">
-        <v>117</v>
-      </c>
-      <c r="J5" t="s">
-        <v>113</v>
-      </c>
-      <c r="K5" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>85</v>
+        <v>175</v>
       </c>
       <c r="F6" t="s">
+        <v>95</v>
+      </c>
+      <c r="G6" t="s">
+        <v>101</v>
+      </c>
+      <c r="H6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I6" t="s">
         <v>103</v>
-      </c>
-      <c r="G6" t="s">
-        <v>109</v>
-      </c>
-      <c r="H6" t="s">
-        <v>110</v>
-      </c>
-      <c r="I6" t="s">
-        <v>159</v>
-      </c>
-      <c r="J6" t="s">
-        <v>160</v>
-      </c>
-      <c r="K6" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>176</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>182</v>
       </c>
       <c r="F7" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G7" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="H7" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="I7" t="s">
-        <v>111</v>
+        <v>177</v>
+      </c>
+      <c r="J7" t="s">
+        <v>150</v>
+      </c>
+      <c r="K7" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1947,42 +1986,42 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="D8">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>119</v>
+        <v>183</v>
       </c>
       <c r="F8" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G8" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="H8" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="I8" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="J8" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="K8" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B9" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -1994,16 +2033,16 @@
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G9" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="H9" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="I9" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -2011,7 +2050,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
@@ -2020,25 +2059,25 @@
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F10" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G10" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="H10" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="I10" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="J10" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="K10" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -2046,34 +2085,34 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>83</v>
+        <v>184</v>
       </c>
       <c r="F11" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G11" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="H11" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" t="s">
+        <v>148</v>
+      </c>
+      <c r="J11" t="s">
         <v>102</v>
       </c>
-      <c r="I11" t="s">
-        <v>157</v>
-      </c>
-      <c r="J11" t="s">
-        <v>110</v>
-      </c>
       <c r="K11" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -2081,7 +2120,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -2090,33 +2129,33 @@
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F12" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G12" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="H12" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="I12" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="J12" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="K12" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
@@ -2125,25 +2164,25 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F13" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G13" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="H13" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="I13" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="J13" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="K13" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -2151,7 +2190,7 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -2160,138 +2199,138 @@
         <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F14" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G14" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="H14" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="I14" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="J14" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="K14" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>44</v>
+        <v>179</v>
       </c>
       <c r="F15" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G15" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="H15" t="s">
+        <v>145</v>
+      </c>
+      <c r="I15" t="s">
+        <v>40</v>
+      </c>
+      <c r="J15" t="s">
         <v>154</v>
       </c>
-      <c r="I15" t="s">
-        <v>42</v>
-      </c>
-      <c r="J15" t="s">
-        <v>165</v>
-      </c>
       <c r="K15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F16" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G16" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="H16" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="I16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J16" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="K16" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F17" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G17" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="H17" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="I17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J17" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="K17" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="B18" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C18" t="s">
         <v>13</v>
@@ -2300,16 +2339,16 @@
         <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F18" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="G18" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H18" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="I18">
         <v>1770911</v>
@@ -2317,60 +2356,60 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F19" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G19" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H19" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="I19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F20" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H20" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="I20" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -2378,7 +2417,7 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C21" t="s">
         <v>18</v>
@@ -2390,178 +2429,265 @@
         <v>19</v>
       </c>
       <c r="F21" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G21" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="H21" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="I21" t="s">
         <v>17</v>
       </c>
       <c r="J21" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="K21" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>87</v>
+        <v>164</v>
       </c>
       <c r="F22" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G22" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="H22" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="I22" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="J22" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="K22" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>161</v>
       </c>
       <c r="B23" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>163</v>
       </c>
       <c r="D23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>88</v>
+        <v>170</v>
       </c>
       <c r="F23" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G23" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="H23" t="s">
-        <v>133</v>
+        <v>167</v>
       </c>
       <c r="I23" t="s">
-        <v>45</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>166</v>
       </c>
       <c r="B24" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>52</v>
+        <v>169</v>
       </c>
       <c r="F24" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G24" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="H24" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="I24" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>172</v>
       </c>
       <c r="B25" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
       <c r="C25" t="s">
-        <v>48</v>
+        <v>163</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>49</v>
+        <v>174</v>
       </c>
       <c r="F25" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G25" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="H25" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="I25" t="s">
-        <v>47</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B26" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="D26">
         <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F26" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G26" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="H26" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="I26" t="s">
-        <v>29</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" t="s">
+        <v>140</v>
+      </c>
+      <c r="C27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F27" t="s">
+        <v>95</v>
+      </c>
+      <c r="G27" t="s">
+        <v>55</v>
+      </c>
+      <c r="H27" t="s">
+        <v>128</v>
+      </c>
+      <c r="I27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" t="s">
+        <v>141</v>
+      </c>
+      <c r="C28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" t="s">
+        <v>95</v>
+      </c>
+      <c r="G28" t="s">
+        <v>55</v>
+      </c>
+      <c r="H28" t="s">
+        <v>127</v>
+      </c>
+      <c r="I28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>125</v>
+      </c>
+      <c r="C29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29" t="s">
+        <v>79</v>
+      </c>
+      <c r="F29" t="s">
+        <v>95</v>
+      </c>
+      <c r="G29" t="s">
+        <v>113</v>
+      </c>
+      <c r="H29" t="s">
+        <v>126</v>
+      </c>
+      <c r="I29" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:E27">
-    <sortCondition ref="E1:E27"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:E30">
+    <sortCondition ref="E1:E30"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:M1"/>

</xml_diff>